<commit_message>
testing. We're getting closer to finish tests
</commit_message>
<xml_diff>
--- a/test/test_files.xlsx
+++ b/test/test_files.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Filename</t>
   </si>
@@ -32,9 +32,6 @@
     <t>basiert auf</t>
   </si>
   <si>
-    <t>f1</t>
-  </si>
-  <si>
     <t>grid</t>
   </si>
   <si>
@@ -59,15 +56,6 @@
     <t>f5</t>
   </si>
   <si>
-    <t>f2</t>
-  </si>
-  <si>
-    <t>f3</t>
-  </si>
-  <si>
-    <t>f4</t>
-  </si>
-  <si>
     <t>timeSeries</t>
   </si>
   <si>
@@ -111,6 +99,15 @@
   </si>
   <si>
     <t>unsupported variable "bla"</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>alles falsch</t>
   </si>
 </sst>
 </file>
@@ -431,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -455,10 +452,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -466,121 +463,135 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>